<commit_message>
updated fileUploadService,test data excel sheets
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCaseFile/BankAccountTestCases.xlsx
+++ b/src/main/resources/TestCaseFile/BankAccountTestCases.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="JavaFile TestCase" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,17 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
-  <si>
-    <t>Method_Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Inputs</t>
   </si>
   <si>
-    <t>ExpectedOutput</t>
-  </si>
-  <si>
     <t>checkMinBalance</t>
   </si>
   <si>
@@ -49,6 +43,18 @@
   </si>
   <si>
     <t>[-1001]</t>
+  </si>
+  <si>
+    <t>Invalid balance amount: Balance amount should be a positive number</t>
+  </si>
+  <si>
+    <t>Method Name</t>
+  </si>
+  <si>
+    <t>Expected Output</t>
+  </si>
+  <si>
+    <t>Expected Status Code</t>
   </si>
 </sst>
 </file>
@@ -84,8 +90,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,75 +375,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.453125" customWidth="1"/>
-    <col min="3" max="3" width="53.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
+      <c r="D5">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>